<commit_message>
Validacion 10 oct 2019
</commit_message>
<xml_diff>
--- a/CONTROL DE INCONSISTENCIAS DTTO 20.xlsx
+++ b/CONTROL DE INCONSISTENCIAS DTTO 20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antonio.hernandezalv\Documents\GitHub\hello-world2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6F99A5-DC56-4629-A24E-FF1B9AFAC0B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E4D7CB8-13E7-409F-904C-6769B45C6DB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="34">
   <si>
     <t>INSTITUTO NACIONAL ELECTORAL</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>JOSÉ CLEMENTE REYNA MENDIOZA</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>MAL POSESIONADO O MAL DIGITALIZADO</t>
   </si>
 </sst>
 </file>
@@ -281,7 +287,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -317,6 +323,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -332,14 +347,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="5" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -858,8 +870,8 @@
   </sheetPr>
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A35" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -871,7 +883,7 @@
     <col min="5" max="5" width="11.54296875" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.1796875" style="2" customWidth="1"/>
     <col min="7" max="7" width="11.54296875" style="2"/>
-    <col min="8" max="8" width="36.6328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="40.6328125" style="2" customWidth="1"/>
     <col min="9" max="9" width="13.81640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="12" style="2" customWidth="1"/>
     <col min="11" max="11" width="11.54296875" style="2"/>
@@ -890,38 +902,38 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.4">
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="I3" s="16" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="I3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="14"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="17"/>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -945,16 +957,16 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -1132,15 +1144,15 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" s="20" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+    <row r="18" spans="1:8" s="15" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
@@ -1282,15 +1294,15 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" s="20" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+    <row r="29" spans="1:8" s="15" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="10"/>
@@ -1432,15 +1444,15 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" s="20" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
+    <row r="40" spans="1:8" s="15" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="10"/>
@@ -1471,7 +1483,9 @@
       <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="11"/>
+      <c r="A43" s="21">
+        <v>43748</v>
+      </c>
       <c r="B43" s="9" t="s">
         <v>16</v>
       </c>
@@ -1562,11 +1576,15 @@
       <c r="C49" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D49" s="8"/>
+      <c r="D49" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
+      <c r="H49" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="12"/>
@@ -1579,18 +1597,20 @@
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
+      <c r="G50" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" s="20" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
+    <row r="51" spans="1:8" s="15" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="13"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="10"/>

</xml_diff>

<commit_message>
CONTROL DE INCONSISTENCIAS DTTO 20.XLSX
INCONSISTENCIAS DTTO 20
</commit_message>
<xml_diff>
--- a/CONTROL DE INCONSISTENCIAS DTTO 20.xlsx
+++ b/CONTROL DE INCONSISTENCIAS DTTO 20.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antonio.hernandezalv\Documents\GitHub\hello-world2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5E8A31-C08B-42BF-A57D-B73BAEFEE6E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{330FC830-2D77-4F24-B67B-737B765D10AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1ERA 7-11 OCT 2019" sheetId="7" r:id="rId1"/>
+    <sheet name="2DA 14-18 OCT 2019" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'1ERA 7-11 OCT 2019'!$A$1:$H$61</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="41">
   <si>
     <t>INSTITUTO NACIONAL ELECTORAL</t>
   </si>
@@ -145,6 +146,22 @@
   <si>
     <t xml:space="preserve">MAL POSESIONADO O MAL DIGITALIZADO, MI SUCIA O
  CON MARCAS </t>
+  </si>
+  <si>
+    <t>HUELLAS CAPTADAS PARCIALMENTE</t>
+  </si>
+  <si>
+    <t>HUELLA CORTADA</t>
+  </si>
+  <si>
+    <t>DF MAL CUADRADO, HUELLAS 
+AUSENTE CON LEYENDA,CAPTADAS PARCIALMENTE</t>
+  </si>
+  <si>
+    <t>HUELLAS AUSENTE SIN LEYENDA, INCLUYE FALANGE</t>
+  </si>
+  <si>
+    <t>HUELLAS ILEGIBLES</t>
   </si>
 </sst>
 </file>
@@ -301,7 +318,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -352,6 +369,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -368,7 +388,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -585,6 +608,233 @@
         <a:xfrm>
           <a:off x="300990" y="270510"/>
           <a:ext cx="1360170" cy="428100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>155685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{588169C1-272D-48CF-9A11-168F1ACC06A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="53340" y="257810"/>
+          <a:ext cx="1404620" cy="424925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>155685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F27F2C58-5CAB-4978-BC4A-B904AD6E5B3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="53340" y="257810"/>
+          <a:ext cx="1404620" cy="424925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>155685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD3C6315-CE8A-44DC-B52A-34BCFC3D4F43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="53340" y="257810"/>
+          <a:ext cx="1404620" cy="424925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -887,8 +1137,8 @@
   </sheetPr>
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A40" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -919,38 +1169,38 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.4">
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="I3" s="21" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="I3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="19"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="20"/>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -974,16 +1224,16 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -1545,7 +1795,7 @@
       <c r="G45" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="18" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1605,7 +1855,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="23" t="s">
+      <c r="H49" s="18" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1623,7 +1873,7 @@
       <c r="G50" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H50" s="23" t="s">
+      <c r="H50" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1791,4 +2041,920 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309CBDC2-4974-49D6-857A-38E008B0EC75}">
+  <dimension ref="A1:H61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="7.90625" customWidth="1"/>
+    <col min="3" max="3" width="45.7265625" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875"/>
+    <col min="8" max="8" width="40.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="B10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="16">
+        <v>43752</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="11"/>
+      <c r="B12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="11"/>
+      <c r="B14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="11"/>
+      <c r="B15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="11"/>
+      <c r="B16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="10"/>
+      <c r="B19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="11"/>
+      <c r="B20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="11"/>
+      <c r="B21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="16">
+        <v>43753</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" ht="20" x14ac:dyDescent="0.35">
+      <c r="A23" s="11"/>
+      <c r="B23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="11"/>
+      <c r="B24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="11"/>
+      <c r="B25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="11"/>
+      <c r="B26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="11"/>
+      <c r="B27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="12"/>
+      <c r="B28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="10"/>
+      <c r="B30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="11"/>
+      <c r="B31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="11"/>
+      <c r="B32" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="11"/>
+      <c r="B34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="11"/>
+      <c r="B35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="11"/>
+      <c r="B36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="11"/>
+      <c r="B37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="11"/>
+      <c r="B38" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="12"/>
+      <c r="B39" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="14"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="8"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="11"/>
+      <c r="B42" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="11"/>
+      <c r="B44" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="11"/>
+      <c r="B45" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="11"/>
+      <c r="B46" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="11"/>
+      <c r="B47" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="11"/>
+      <c r="B48" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="11"/>
+      <c r="B49" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="12"/>
+      <c r="B50" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="13"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="10"/>
+      <c r="B52" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="8"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="11"/>
+      <c r="B53" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="8"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="11"/>
+      <c r="B54" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="8"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="11"/>
+      <c r="B55" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="8"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="11"/>
+      <c r="B56" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="8"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="11"/>
+      <c r="B57" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="8"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="11"/>
+      <c r="B58" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="8"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="11"/>
+      <c r="B59" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="8"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="11"/>
+      <c r="B60" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="8"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="12"/>
+      <c r="B61" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="A6:H6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CONTROL DE INCIDENCIAS DTTO 20.XLSX
SIIAPE VALIDADCION 161019
</commit_message>
<xml_diff>
--- a/CONTROL DE INCONSISTENCIAS DTTO 20.xlsx
+++ b/CONTROL DE INCONSISTENCIAS DTTO 20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antonio.hernandezalv\Documents\GitHub\hello-world2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{330FC830-2D77-4F24-B67B-737B765D10AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D218C69C-F339-4F05-946C-8F481E2A7F6D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="44">
   <si>
     <t>INSTITUTO NACIONAL ELECTORAL</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>HUELLAS ILEGIBLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUELLAS CAPTADA PARCIRCIALMENTE </t>
+  </si>
+  <si>
+    <t>HULLAS CAPTADAS PARCIALMENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HUELLAS CAPTADA PARCIRCIALMENTE, HUELLAS AUSENTE CON LEYENDA, MI ACTA DAÑADA</t>
   </si>
 </sst>
 </file>
@@ -372,6 +381,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,12 +401,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1169,38 +1178,38 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.4">
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="I3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="20"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="22"/>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1224,16 +1233,16 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -2047,8 +2056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309CBDC2-4974-49D6-857A-38E008B0EC75}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2087,24 +2096,24 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -2118,16 +2127,16 @@
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
@@ -2241,7 +2250,7 @@
       <c r="G13" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="19" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2259,7 +2268,7 @@
       <c r="G14" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="19" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2291,7 +2300,7 @@
       <c r="G16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="19" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2309,7 +2318,7 @@
       <c r="G17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="19" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2317,10 +2326,10 @@
       <c r="A18" s="13"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2415,7 +2424,7 @@
       <c r="G24" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="19" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2433,7 +2442,7 @@
       <c r="G25" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="24" t="s">
+      <c r="H25" s="19" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2483,10 +2492,10 @@
       <c r="A29" s="13"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -2532,7 +2541,9 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
+      <c r="A33" s="16">
+        <v>43754</v>
+      </c>
       <c r="B33" s="9" t="s">
         <v>18</v>
       </c>
@@ -2633,10 +2644,10 @@
       <c r="A40" s="13"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2680,8 +2691,12 @@
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="8"/>
+      <c r="G43" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="11"/>
@@ -2694,10 +2709,14 @@
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G44" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="20" x14ac:dyDescent="0.35">
       <c r="A45" s="11"/>
       <c r="B45" s="9" t="s">
         <v>20</v>
@@ -2705,16 +2724,18 @@
       <c r="C45" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="17"/>
+      <c r="D45" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="E45" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="17" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -2799,10 +2820,10 @@
       <c r="A51" s="13"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
       <c r="H51" s="14" t="s">
         <v>11</v>
       </c>

</xml_diff>